<commit_message>
[MOSIP-14369] Default data removed.
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/upload/xlsx/machine_spec.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/upload/xlsx/machine_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -47,27 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">is_active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vostro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To take enrollments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eng</t>
   </si>
 </sst>
 </file>
@@ -158,25 +137,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -196,110 +167,47 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576 1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.43"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>3568</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>1.454</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>3568</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>1.454</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>